<commit_message>
Add strucchange::breakpoints to package comparison
</commit_message>
<xml_diff>
--- a/man/figures/packages_tables.xlsx
+++ b/man/figures/packages_tables.xlsx
@@ -156,7 +156,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="82">
   <si>
     <t>ecp</t>
   </si>
@@ -396,6 +396,12 @@
   </si>
   <si>
     <t>Prior</t>
+  </si>
+  <si>
+    <t>strucchange::breakpoints</t>
+  </si>
+  <si>
+    <t>BIC</t>
   </si>
 </sst>
 </file>
@@ -965,15 +971,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M32"/>
+  <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.42578125" style="38" customWidth="1"/>
     <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
@@ -1140,28 +1146,28 @@
     </row>
     <row r="5" spans="1:13" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="B5" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="15" t="s">
         <v>10</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="F5" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="33" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="34" t="s">
+        <v>10</v>
       </c>
       <c r="H5" s="26" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="I5" s="14" t="s">
         <v>11</v>
@@ -1181,19 +1187,19 @@
     </row>
     <row r="6" spans="1:13" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B6" s="31" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>24</v>
+        <v>21</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>28</v>
       </c>
       <c r="D6" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="17" t="s">
-        <v>10</v>
+      <c r="E6" s="15" t="s">
+        <v>60</v>
       </c>
       <c r="F6" s="17" t="s">
         <v>10</v>
@@ -1222,13 +1228,13 @@
     </row>
     <row r="7" spans="1:13" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B7" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>25</v>
+        <v>16</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>24</v>
       </c>
       <c r="D7" s="17" t="s">
         <v>10</v>
@@ -1239,8 +1245,8 @@
       <c r="F7" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="32" t="s">
-        <v>10</v>
+      <c r="G7" s="33" t="s">
+        <v>11</v>
       </c>
       <c r="H7" s="26" t="s">
         <v>15</v>
@@ -1251,8 +1257,8 @@
       <c r="J7" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="K7" s="14" t="s">
-        <v>11</v>
+      <c r="K7" s="17" t="s">
+        <v>10</v>
       </c>
       <c r="L7" s="32" t="s">
         <v>10</v>
@@ -1263,13 +1269,13 @@
     </row>
     <row r="8" spans="1:13" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>49</v>
+        <v>2</v>
       </c>
       <c r="B8" s="31" t="s">
-        <v>50</v>
+        <v>9</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="D8" s="17" t="s">
         <v>10</v>
@@ -1283,7 +1289,7 @@
       <c r="G8" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="28" t="s">
+      <c r="H8" s="26" t="s">
         <v>15</v>
       </c>
       <c r="I8" s="14" t="s">
@@ -1292,8 +1298,8 @@
       <c r="J8" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="K8" s="15" t="s">
-        <v>60</v>
+      <c r="K8" s="14" t="s">
+        <v>11</v>
       </c>
       <c r="L8" s="32" t="s">
         <v>10</v>
@@ -1304,13 +1310,13 @@
     </row>
     <row r="9" spans="1:13" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="B9" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>27</v>
+        <v>50</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>53</v>
       </c>
       <c r="D9" s="17" t="s">
         <v>10</v>
@@ -1324,8 +1330,8 @@
       <c r="G9" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="H9" s="29" t="s">
-        <v>34</v>
+      <c r="H9" s="28" t="s">
+        <v>15</v>
       </c>
       <c r="I9" s="14" t="s">
         <v>11</v>
@@ -1333,8 +1339,8 @@
       <c r="J9" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="K9" s="17" t="s">
-        <v>10</v>
+      <c r="K9" s="15" t="s">
+        <v>60</v>
       </c>
       <c r="L9" s="32" t="s">
         <v>10</v>
@@ -1345,28 +1351,28 @@
     </row>
     <row r="10" spans="1:13" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B10" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>28</v>
+        <v>22</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>27</v>
       </c>
       <c r="D10" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="14" t="s">
-        <v>11</v>
+      <c r="E10" s="17" t="s">
+        <v>10</v>
       </c>
       <c r="F10" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="H10" s="26" t="s">
-        <v>15</v>
+      <c r="G10" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="29" t="s">
+        <v>34</v>
       </c>
       <c r="I10" s="14" t="s">
         <v>11</v>
@@ -1386,25 +1392,25 @@
     </row>
     <row r="11" spans="1:13" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="B11" s="31" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="E11" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="G11" s="34" t="s">
-        <v>10</v>
+        <v>20</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="33" t="s">
+        <v>11</v>
       </c>
       <c r="H11" s="26" t="s">
         <v>15</v>
@@ -1412,34 +1418,34 @@
       <c r="I11" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="J11" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="K11" s="14" t="s">
-        <v>11</v>
+      <c r="J11" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="K11" s="17" t="s">
+        <v>10</v>
       </c>
       <c r="L11" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="M11" s="15" t="s">
+      <c r="M11" s="17" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:13" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B12" s="31" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" s="14" t="s">
-        <v>59</v>
+        <v>41</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>10</v>
       </c>
       <c r="F12" s="15" t="s">
         <v>10</v>
@@ -1468,19 +1474,19 @@
     </row>
     <row r="13" spans="1:13" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B13" s="31" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="D13" s="15" t="s">
         <v>10</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>11</v>
+        <v>59</v>
       </c>
       <c r="F13" s="15" t="s">
         <v>10</v>
@@ -1497,8 +1503,8 @@
       <c r="J13" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="K13" s="15" t="s">
-        <v>10</v>
+      <c r="K13" s="14" t="s">
+        <v>11</v>
       </c>
       <c r="L13" s="32" t="s">
         <v>10</v>
@@ -1508,8 +1514,45 @@
       </c>
     </row>
     <row r="14" spans="1:13" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="6"/>
-      <c r="H14" s="6"/>
+      <c r="A14" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="H14" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="I14" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="J14" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="K14" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="L14" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="M14" s="15" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="15" spans="1:13" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="6"/>
@@ -1535,9 +1578,9 @@
       <c r="B20" s="6"/>
       <c r="H20" s="6"/>
     </row>
-    <row r="21" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21"/>
-      <c r="B21" s="2"/>
+    <row r="21" spans="1:8" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="6"/>
+      <c r="H21" s="6"/>
     </row>
     <row r="22" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22"/>
@@ -1559,12 +1602,16 @@
       <c r="A26"/>
       <c r="B26" s="2"/>
     </row>
-    <row r="27" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27"/>
+      <c r="B27" s="2"/>
+    </row>
     <row r="28" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="29" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="30" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="31" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="32" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:B1"/>
@@ -1579,10 +1626,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K25"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1720,55 +1767,55 @@
     </row>
     <row r="5" spans="1:11" s="22" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="B5" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5" s="17" t="s">
-        <v>10</v>
+        <v>22</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>11</v>
       </c>
       <c r="I5" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="17" t="s">
-        <v>10</v>
+      <c r="J5" s="14" t="s">
+        <v>81</v>
       </c>
       <c r="K5" s="23"/>
     </row>
     <row r="6" spans="1:11" s="22" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B6" s="31" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C6" s="17" t="s">
         <v>10</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="E6" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="14" t="s">
-        <v>11</v>
+      <c r="F6" s="17" t="s">
+        <v>10</v>
       </c>
       <c r="G6" s="32" t="s">
         <v>10</v>
@@ -1786,16 +1833,16 @@
     </row>
     <row r="7" spans="1:11" s="22" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B7" s="31" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C7" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="14" t="s">
-        <v>11</v>
+      <c r="D7" s="17" t="s">
+        <v>17</v>
       </c>
       <c r="E7" s="17" t="s">
         <v>10</v>
@@ -1819,22 +1866,22 @@
     </row>
     <row r="8" spans="1:11" s="22" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>49</v>
+        <v>2</v>
       </c>
       <c r="B8" s="31" t="s">
-        <v>50</v>
+        <v>9</v>
       </c>
       <c r="C8" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="17" t="s">
-        <v>10</v>
+      <c r="D8" s="14" t="s">
+        <v>11</v>
       </c>
       <c r="E8" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="17" t="s">
-        <v>10</v>
+      <c r="F8" s="14" t="s">
+        <v>11</v>
       </c>
       <c r="G8" s="32" t="s">
         <v>10</v>
@@ -1852,10 +1899,10 @@
     </row>
     <row r="9" spans="1:11" s="22" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="B9" s="31" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="C9" s="17" t="s">
         <v>10</v>
@@ -1866,8 +1913,8 @@
       <c r="E9" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="14" t="s">
-        <v>11</v>
+      <c r="F9" s="17" t="s">
+        <v>10</v>
       </c>
       <c r="G9" s="32" t="s">
         <v>10</v>
@@ -1885,10 +1932,10 @@
     </row>
     <row r="10" spans="1:11" s="22" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B10" s="31" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C10" s="17" t="s">
         <v>10</v>
@@ -1899,8 +1946,8 @@
       <c r="E10" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="17" t="s">
-        <v>10</v>
+      <c r="F10" s="14" t="s">
+        <v>11</v>
       </c>
       <c r="G10" s="32" t="s">
         <v>10</v>
@@ -1918,9 +1965,11 @@
     </row>
     <row r="11" spans="1:11" s="22" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="B11" s="32"/>
+        <v>23</v>
+      </c>
+      <c r="B11" s="31" t="s">
+        <v>20</v>
+      </c>
       <c r="C11" s="17" t="s">
         <v>10</v>
       </c>
@@ -1930,7 +1979,7 @@
       <c r="E11" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="15" t="s">
+      <c r="F11" s="17" t="s">
         <v>10</v>
       </c>
       <c r="G11" s="32" t="s">
@@ -1949,22 +1998,20 @@
     </row>
     <row r="12" spans="1:11" s="22" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="B12" s="31" t="s">
-        <v>47</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="B12" s="32"/>
       <c r="C12" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="14" t="s">
-        <v>11</v>
+      <c r="D12" s="17" t="s">
+        <v>10</v>
       </c>
       <c r="E12" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="14" t="s">
-        <v>11</v>
+      <c r="F12" s="15" t="s">
+        <v>10</v>
       </c>
       <c r="G12" s="32" t="s">
         <v>10</v>
@@ -1976,46 +2023,75 @@
         <v>10</v>
       </c>
       <c r="J12" s="17" t="s">
-        <v>55</v>
+        <v>10</v>
       </c>
       <c r="K12" s="23"/>
     </row>
     <row r="13" spans="1:11" s="22" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="H13" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="I13" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="J13" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="K13" s="23"/>
+    </row>
+    <row r="14" spans="1:11" s="22" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="31" t="s">
+      <c r="B14" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="C13" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="G13" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="H13" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="I13" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="J13" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="K13" s="23"/>
-    </row>
-    <row r="14" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="6"/>
-      <c r="K14" s="5"/>
+      <c r="C14" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="H14" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="I14" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="J14" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="K14" s="23"/>
     </row>
     <row r="15" spans="1:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="6"/>
@@ -2057,7 +2133,11 @@
       <c r="B24" s="6"/>
       <c r="K24" s="5"/>
     </row>
-    <row r="25" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="2:11" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="6"/>
+      <c r="K25" s="5"/>
+    </row>
+    <row r="26" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update vignettes with Dirichlet prior
</commit_message>
<xml_diff>
--- a/man/figures/packages_tables.xlsx
+++ b/man/figures/packages_tables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="35085" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="35085"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -445,9 +445,6 @@
     <t>auto: slope + int</t>
   </si>
   <si>
-    <t>auto: int</t>
-  </si>
-  <si>
     <t>specify: slope</t>
   </si>
   <si>
@@ -529,9 +526,6 @@
     <t>2.0.0</t>
   </si>
   <si>
-    <t>auto: int?</t>
-  </si>
-  <si>
     <t>AIC and deviance</t>
   </si>
   <si>
@@ -547,9 +541,6 @@
     <t>AR(N)</t>
   </si>
   <si>
-    <t>AR(2)</t>
-  </si>
-  <si>
     <t>?</t>
   </si>
   <si>
@@ -617,6 +608,15 @@
   </si>
   <si>
     <t>hyper</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>int?</t>
+  </si>
+  <si>
+    <t>AR(&lt;=2)</t>
   </si>
 </sst>
 </file>
@@ -1182,8 +1182,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C33" sqref="C33:C36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1213,62 +1213,62 @@
       </c>
       <c r="B1" s="41"/>
       <c r="C1" s="40" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D1" s="40"/>
       <c r="E1" s="40"/>
       <c r="F1" s="40"/>
       <c r="G1" s="41"/>
       <c r="H1" s="42" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="I1" s="40"/>
       <c r="J1" s="40"/>
       <c r="K1" s="40"/>
       <c r="L1" s="41"/>
       <c r="M1" s="24" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B2" s="30" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>12</v>
       </c>
       <c r="E2" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="F2" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="G2" s="30" t="s">
+      <c r="H2" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="I2" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="J2" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="L2" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="I2" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="L2" s="30" t="s">
-        <v>72</v>
-      </c>
       <c r="M2" s="18" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:13" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -1276,16 +1276,16 @@
         <v>3</v>
       </c>
       <c r="B3" s="31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F3" s="25" t="s">
         <v>13</v>
@@ -1320,13 +1320,13 @@
         <v>20</v>
       </c>
       <c r="C4" s="38" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F4" s="14" t="s">
         <v>11</v>
@@ -1355,13 +1355,13 @@
     </row>
     <row r="5" spans="1:13" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B5" s="31" t="s">
         <v>22</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D5" s="15" t="s">
         <v>10</v>
@@ -1402,13 +1402,13 @@
         <v>21</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>28</v>
+        <v>80</v>
       </c>
       <c r="D6" s="17" t="s">
         <v>10</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F6" s="17" t="s">
         <v>10</v>
@@ -1425,8 +1425,8 @@
       <c r="J6" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="K6" s="17" t="s">
-        <v>10</v>
+      <c r="K6" s="14" t="s">
+        <v>11</v>
       </c>
       <c r="L6" s="32" t="s">
         <v>10</v>
@@ -1484,7 +1484,7 @@
         <v>9</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>25</v>
+        <v>80</v>
       </c>
       <c r="D8" s="17" t="s">
         <v>10</v>
@@ -1519,13 +1519,13 @@
     </row>
     <row r="9" spans="1:13" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="B9" s="31" t="s">
-        <v>50</v>
-      </c>
       <c r="C9" s="16" t="s">
-        <v>53</v>
+        <v>81</v>
       </c>
       <c r="D9" s="17" t="s">
         <v>10</v>
@@ -1549,7 +1549,7 @@
         <v>10</v>
       </c>
       <c r="K9" s="15" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="L9" s="32" t="s">
         <v>10</v>
@@ -1566,7 +1566,7 @@
         <v>22</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D10" s="17" t="s">
         <v>10</v>
@@ -1581,7 +1581,7 @@
         <v>10</v>
       </c>
       <c r="H10" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I10" s="14" t="s">
         <v>11</v>
@@ -1607,7 +1607,7 @@
         <v>20</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D11" s="17" t="s">
         <v>10</v>
@@ -1642,16 +1642,16 @@
     </row>
     <row r="12" spans="1:13" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="31" t="s">
+      <c r="C12" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D12" s="15" t="s">
         <v>40</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>41</v>
       </c>
       <c r="E12" s="15" t="s">
         <v>10</v>
@@ -1683,19 +1683,19 @@
     </row>
     <row r="13" spans="1:13" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="31" t="s">
+      <c r="C13" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="13" t="s">
-        <v>48</v>
-      </c>
       <c r="D13" s="15" t="s">
         <v>10</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>59</v>
+        <v>82</v>
       </c>
       <c r="F13" s="15" t="s">
         <v>10</v>
@@ -1724,13 +1724,13 @@
     </row>
     <row r="14" spans="1:13" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="B14" s="31" t="s">
-        <v>52</v>
-      </c>
       <c r="C14" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D14" s="15" t="s">
         <v>10</v>
@@ -1838,7 +1838,7 @@
   <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1862,14 +1862,14 @@
       </c>
       <c r="B1" s="41"/>
       <c r="C1" s="40" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D1" s="40"/>
       <c r="E1" s="40"/>
       <c r="F1" s="40"/>
       <c r="G1" s="41"/>
       <c r="H1" s="40" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I1" s="40"/>
       <c r="J1" s="40"/>
@@ -1877,34 +1877,34 @@
     </row>
     <row r="2" spans="1:11" s="22" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B2" s="30" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>5</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>6</v>
       </c>
       <c r="G2" s="30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H2" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="J2" s="8" t="s">
         <v>37</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>38</v>
       </c>
       <c r="K2" s="21"/>
     </row>
@@ -1913,7 +1913,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" s="14" t="s">
         <v>11</v>
@@ -1937,7 +1937,7 @@
         <v>11</v>
       </c>
       <c r="J3" s="14" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="K3" s="23"/>
     </row>
@@ -1964,19 +1964,19 @@
         <v>11</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I4" s="17" t="s">
         <v>10</v>
       </c>
       <c r="J4" s="14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="K4" s="23"/>
     </row>
     <row r="5" spans="1:11" s="22" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B5" s="31" t="s">
         <v>22</v>
@@ -2003,7 +2003,7 @@
         <v>10</v>
       </c>
       <c r="J5" s="14" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K5" s="23"/>
     </row>
@@ -2108,10 +2108,10 @@
     </row>
     <row r="9" spans="1:11" s="22" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="31" t="s">
         <v>49</v>
-      </c>
-      <c r="B9" s="31" t="s">
-        <v>50</v>
       </c>
       <c r="C9" s="17" t="s">
         <v>10</v>
@@ -2207,7 +2207,7 @@
     </row>
     <row r="12" spans="1:11" s="22" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B12" s="32"/>
       <c r="C12" s="17" t="s">
@@ -2238,11 +2238,11 @@
     </row>
     <row r="13" spans="1:11" s="22" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="31" t="s">
-        <v>47</v>
-      </c>
       <c r="C13" s="17" t="s">
         <v>10</v>
       </c>
@@ -2265,16 +2265,16 @@
         <v>10</v>
       </c>
       <c r="J13" s="17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="K13" s="23"/>
     </row>
     <row r="14" spans="1:11" s="22" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="31" t="s">
         <v>51</v>
-      </c>
-      <c r="B14" s="31" t="s">
-        <v>52</v>
       </c>
       <c r="C14" s="17" t="s">
         <v>10</v>
@@ -2363,8 +2363,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2381,7 +2381,7 @@
       </c>
       <c r="B1" s="41"/>
       <c r="C1" s="40" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D1" s="40"/>
       <c r="E1" s="40"/>
@@ -2390,25 +2390,25 @@
     </row>
     <row r="2" spans="1:10" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B2" s="30" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>44</v>
-      </c>
       <c r="F2" s="18" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
@@ -2419,7 +2419,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="36" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>11</v>
@@ -2431,7 +2431,7 @@
         <v>11</v>
       </c>
       <c r="F3" s="35" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G3" s="10" t="s">
         <v>11</v>
@@ -2457,7 +2457,7 @@
         <v>10</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G4" s="11" t="s">
         <v>10</v>
@@ -2468,7 +2468,7 @@
     </row>
     <row r="5" spans="1:10" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B5" s="31" t="s">
         <v>22</v>
@@ -2483,7 +2483,7 @@
         <v>10</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G5" s="11" t="s">
         <v>10</v>
@@ -2509,7 +2509,7 @@
         <v>10</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G6" s="11" t="s">
         <v>10</v>
@@ -2535,10 +2535,10 @@
         <v>10</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G7" s="39" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -2561,7 +2561,7 @@
         <v>10</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G8" s="11" t="s">
         <v>10</v>
@@ -2572,11 +2572,11 @@
     </row>
     <row r="9" spans="1:10" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="B9" s="36" t="s">
-        <v>50</v>
-      </c>
       <c r="C9" s="11" t="s">
         <v>10</v>
       </c>
@@ -2587,7 +2587,7 @@
         <v>10</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G9" s="11" t="s">
         <v>10</v>
@@ -2613,7 +2613,7 @@
         <v>10</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G10" s="11" t="s">
         <v>10</v>
@@ -2639,7 +2639,7 @@
         <v>10</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G11" s="11" t="s">
         <v>10</v>
@@ -2650,11 +2650,11 @@
     </row>
     <row r="12" spans="1:10" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="36" t="s">
-        <v>40</v>
-      </c>
       <c r="C12" s="11" t="s">
         <v>10</v>
       </c>
@@ -2665,7 +2665,7 @@
         <v>10</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G12" s="11" t="s">
         <v>10</v>
@@ -2676,11 +2676,11 @@
     </row>
     <row r="13" spans="1:10" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="36" t="s">
-        <v>47</v>
-      </c>
       <c r="C13" s="11" t="s">
         <v>10</v>
       </c>
@@ -2691,7 +2691,7 @@
         <v>10</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G13" s="11" t="s">
         <v>10</v>
@@ -2702,11 +2702,11 @@
     </row>
     <row r="14" spans="1:10" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="B14" s="36" t="s">
-        <v>52</v>
-      </c>
       <c r="C14" s="11" t="s">
         <v>10</v>
       </c>
@@ -2717,7 +2717,7 @@
         <v>11</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G14" s="11" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Add empty line and update NEWS
</commit_message>
<xml_diff>
--- a/man/figures/packages_tables.xlsx
+++ b/man/figures/packages_tables.xlsx
@@ -31,7 +31,7 @@
     <author>Jonas Kristoffer Lindeløv</author>
   </authors>
   <commentList>
-    <comment ref="L2" authorId="0" shapeId="0">
+    <comment ref="M2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -55,7 +55,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M2" authorId="0" shapeId="0">
+    <comment ref="N2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -368,7 +368,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="84">
   <si>
     <t>ecp</t>
   </si>
@@ -617,6 +617,9 @@
   </si>
   <si>
     <t>AR(&lt;=2)</t>
+  </si>
+  <si>
+    <t>2+pred</t>
   </si>
 </sst>
 </file>
@@ -661,7 +664,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -689,6 +692,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -771,7 +786,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -894,6 +909,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1180,10 +1201,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M33"/>
+  <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1194,20 +1215,21 @@
     <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.85546875" customWidth="1"/>
-    <col min="13" max="13" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.7109375" customWidth="1"/>
-    <col min="15" max="15" width="10" customWidth="1"/>
-    <col min="16" max="16" width="6.28515625" customWidth="1"/>
-    <col min="17" max="17" width="7" customWidth="1"/>
+    <col min="7" max="7" width="8.28515625" customWidth="1"/>
+    <col min="8" max="8" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.85546875" customWidth="1"/>
+    <col min="14" max="14" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.7109375" customWidth="1"/>
+    <col min="16" max="16" width="10" customWidth="1"/>
+    <col min="17" max="17" width="6.28515625" customWidth="1"/>
+    <col min="18" max="18" width="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A1" s="40" t="s">
         <v>4</v>
       </c>
@@ -1218,19 +1240,20 @@
       <c r="D1" s="40"/>
       <c r="E1" s="40"/>
       <c r="F1" s="40"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="42" t="s">
+      <c r="G1" s="40"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="I1" s="40"/>
       <c r="J1" s="40"/>
       <c r="K1" s="40"/>
-      <c r="L1" s="41"/>
-      <c r="M1" s="24" t="s">
+      <c r="L1" s="40"/>
+      <c r="M1" s="41"/>
+      <c r="N1" s="24" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>54</v>
       </c>
@@ -1249,29 +1272,32 @@
       <c r="F2" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="G2" s="30" t="s">
+      <c r="G2" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="I2" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="I2" s="18" t="s">
+      <c r="J2" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="K2" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="L2" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="L2" s="30" t="s">
+      <c r="M2" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="M2" s="18" t="s">
+      <c r="N2" s="18" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>3</v>
       </c>
@@ -1290,29 +1316,32 @@
       <c r="F3" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="34" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" s="26" t="s">
+      <c r="G3" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="14" t="s">
-        <v>11</v>
-      </c>
       <c r="J3" s="14" t="s">
         <v>11</v>
       </c>
       <c r="K3" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="L3" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="M3" s="14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L3" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="M3" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="N3" s="14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>19</v>
       </c>
@@ -1331,29 +1360,32 @@
       <c r="F4" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" s="27" t="s">
+      <c r="G4" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="J4" s="17" t="s">
-        <v>10</v>
+      <c r="J4" s="14" t="s">
+        <v>11</v>
       </c>
       <c r="K4" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="L4" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="M4" s="17" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L4" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="M4" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="N4" s="17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>77</v>
       </c>
@@ -1372,29 +1404,30 @@
       <c r="F5" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="34" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5" s="26" t="s">
+      <c r="G5" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="44"/>
+      <c r="I5" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="J5" s="17" t="s">
-        <v>10</v>
+      <c r="J5" s="14" t="s">
+        <v>11</v>
       </c>
       <c r="K5" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="M5" s="17" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L5" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="M5" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="N5" s="17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>0</v>
       </c>
@@ -1413,29 +1446,30 @@
       <c r="F6" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="26" t="s">
+      <c r="G6" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="44"/>
+      <c r="I6" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="I6" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="J6" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="K6" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="L6" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="M6" s="17" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J6" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="K6" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="L6" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="M6" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="N6" s="17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>1</v>
       </c>
@@ -1454,29 +1488,30 @@
       <c r="F7" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="H7" s="26" t="s">
+      <c r="G7" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="44"/>
+      <c r="I7" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="I7" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="J7" s="17" t="s">
-        <v>10</v>
+      <c r="J7" s="14" t="s">
+        <v>11</v>
       </c>
       <c r="K7" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="L7" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="M7" s="17" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L7" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="M7" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="N7" s="17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>2</v>
       </c>
@@ -1495,29 +1530,30 @@
       <c r="F8" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="H8" s="26" t="s">
+      <c r="G8" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="44"/>
+      <c r="I8" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="J8" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="K8" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="L8" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="M8" s="17" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J8" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="K8" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="L8" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="M8" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="N8" s="17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>48</v>
       </c>
@@ -1536,29 +1572,30 @@
       <c r="F9" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="H9" s="28" t="s">
+      <c r="G9" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9" s="44"/>
+      <c r="I9" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="I9" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="J9" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="K9" s="15" t="s">
+      <c r="J9" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="K9" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="L9" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="L9" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="M9" s="17" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M9" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="N9" s="17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>18</v>
       </c>
@@ -1577,29 +1614,30 @@
       <c r="F10" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="H10" s="29" t="s">
+      <c r="G10" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="44"/>
+      <c r="I10" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="I10" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="J10" s="17" t="s">
-        <v>10</v>
+      <c r="J10" s="14" t="s">
+        <v>11</v>
       </c>
       <c r="K10" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="L10" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="M10" s="17" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L10" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="M10" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="N10" s="17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>23</v>
       </c>
@@ -1618,29 +1656,30 @@
       <c r="F11" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="H11" s="26" t="s">
+      <c r="G11" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" s="44"/>
+      <c r="I11" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="I11" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="J11" s="17" t="s">
-        <v>10</v>
+      <c r="J11" s="14" t="s">
+        <v>11</v>
       </c>
       <c r="K11" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="L11" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="M11" s="17" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L11" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="M11" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="N11" s="17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>38</v>
       </c>
@@ -1659,29 +1698,30 @@
       <c r="F12" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="G12" s="34" t="s">
-        <v>10</v>
-      </c>
-      <c r="H12" s="26" t="s">
+      <c r="G12" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12" s="44"/>
+      <c r="I12" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="I12" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="J12" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="K12" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="L12" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="M12" s="15" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J12" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="K12" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="L12" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="M12" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="N12" s="15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>45</v>
       </c>
@@ -1700,29 +1740,30 @@
       <c r="F13" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="G13" s="34" t="s">
-        <v>10</v>
-      </c>
-      <c r="H13" s="26" t="s">
+      <c r="G13" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H13" s="44"/>
+      <c r="I13" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="I13" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="J13" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="K13" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="L13" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="M13" s="15" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J13" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="K13" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="L13" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="M13" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="N13" s="15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>50</v>
       </c>
@@ -1741,91 +1782,92 @@
       <c r="F14" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="G14" s="34" t="s">
-        <v>10</v>
-      </c>
-      <c r="H14" s="26" t="s">
+      <c r="G14" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H14" s="44"/>
+      <c r="I14" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="I14" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="J14" s="15" t="s">
-        <v>10</v>
+      <c r="J14" s="14" t="s">
+        <v>11</v>
       </c>
       <c r="K14" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="L14" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="M14" s="15" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L14" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="M14" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="N14" s="15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="6"/>
-      <c r="H15" s="6"/>
-    </row>
-    <row r="16" spans="1:13" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I15" s="6"/>
+    </row>
+    <row r="16" spans="1:14" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="6"/>
-      <c r="H16" s="6"/>
-    </row>
-    <row r="17" spans="1:8" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I16" s="6"/>
+    </row>
+    <row r="17" spans="1:9" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="6"/>
-      <c r="H17" s="6"/>
-    </row>
-    <row r="18" spans="1:8" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I17" s="6"/>
+    </row>
+    <row r="18" spans="1:9" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="6"/>
-      <c r="H18" s="6"/>
-    </row>
-    <row r="19" spans="1:8" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I18" s="6"/>
+    </row>
+    <row r="19" spans="1:9" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="6"/>
-      <c r="H19" s="6"/>
-    </row>
-    <row r="20" spans="1:8" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I19" s="6"/>
+    </row>
+    <row r="20" spans="1:9" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="6"/>
-      <c r="H20" s="6"/>
-    </row>
-    <row r="21" spans="1:8" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I20" s="6"/>
+    </row>
+    <row r="21" spans="1:9" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="6"/>
-      <c r="H21" s="6"/>
-    </row>
-    <row r="22" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I21" s="6"/>
+    </row>
+    <row r="22" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22"/>
       <c r="B22" s="2"/>
     </row>
-    <row r="23" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23"/>
       <c r="B23" s="2"/>
     </row>
-    <row r="24" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24"/>
       <c r="B24" s="2"/>
     </row>
-    <row r="25" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25"/>
       <c r="B25" s="2"/>
     </row>
-    <row r="26" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26"/>
       <c r="B26" s="2"/>
     </row>
-    <row r="27" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27"/>
       <c r="B27" s="2"/>
     </row>
-    <row r="28" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:G1"/>
-    <mergeCell ref="H1:L1"/>
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="I1:M1"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -1838,7 +1880,7 @@
   <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1981,14 +2023,14 @@
       <c r="B5" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>10</v>
+      <c r="C5" s="43" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="43" t="s">
+        <v>57</v>
+      </c>
+      <c r="E5" s="43" t="s">
+        <v>57</v>
       </c>
       <c r="F5" s="15" t="s">
         <v>10</v>

</xml_diff>